<commit_message>
fixing minor bug on norma tintum anak and section 73's answer
</commit_message>
<xml_diff>
--- a/backend/src/data/dummy_questions/dummy_tintum_anak.xlsx
+++ b/backend/src/data/dummy_questions/dummy_tintum_anak.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Important Files\Informatika ISTTS\_Semester 6\Kerja_Praktek\Project\adiputro_psytest_backend\backend\src\data\dummy_questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\adiputro_psytest_backend\backend\src\data\dummy_questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20478F87-2E11-4AB8-B648-A1F0EC976B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC30F60-0614-4754-A2B6-D39C6153DC1F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="15375" windowHeight="7995" tabRatio="754" activeTab="8" xr2:uid="{1C76B0C7-30FC-44AF-999C-E5F402443C8E}"/>
+    <workbookView xWindow="1428" yWindow="1428" windowWidth="15372" windowHeight="7992" tabRatio="754" activeTab="1" xr2:uid="{1C76B0C7-30FC-44AF-999C-E5F402443C8E}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,10 @@
     <sheet name="Keterangan Field" sheetId="4" r:id="rId10"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -755,22 +747,22 @@
       <selection activeCell="B16" sqref="B7:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -805,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -838,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -867,12 +859,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -907,7 +899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -921,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -935,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>79</v>
       </c>
@@ -949,7 +941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -963,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -977,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -991,7 +983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -1005,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -1019,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -1033,7 +1025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>79</v>
       </c>
@@ -1058,24 +1050,24 @@
   <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="77.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1078,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1095,7 +1087,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
@@ -1106,7 +1098,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1117,7 +1109,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1128,7 +1120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
@@ -1139,7 +1131,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
@@ -1150,7 +1142,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1161,7 +1153,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1172,7 +1164,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1183,7 +1175,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1194,7 +1186,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1222,22 +1214,22 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="5" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
@@ -1253,7 +1245,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>49</v>
@@ -1267,7 +1259,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="6" t="s">
         <v>7</v>
@@ -1279,7 +1271,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
         <v>50</v>
@@ -1293,7 +1285,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
         <v>51</v>
@@ -1307,7 +1299,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>52</v>
@@ -1321,7 +1313,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>53</v>
@@ -1335,7 +1327,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
         <v>54</v>
@@ -1349,7 +1341,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>14</v>
@@ -1363,7 +1355,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>18</v>
@@ -1377,7 +1369,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>56</v>
@@ -1391,7 +1383,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -1399,7 +1391,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>67</v>
       </c>
@@ -1407,13 +1399,13 @@
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -1448,7 +1440,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -1463,26 +1455,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2AE856B-9E5B-4C01-896D-625B9683C8E7}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1517,7 +1509,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -1550,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -1579,12 +1571,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -1619,7 +1611,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -1648,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -1677,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>79</v>
       </c>
@@ -1706,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -1735,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -1764,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -1793,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -1822,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -1851,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -1880,7 +1872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>79</v>
       </c>
@@ -1909,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>79</v>
       </c>
@@ -1938,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>79</v>
       </c>
@@ -1967,7 +1959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -1996,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>79</v>
       </c>
@@ -2025,7 +2017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>79</v>
       </c>
@@ -2054,7 +2046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -2083,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>79</v>
       </c>
@@ -2112,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>79</v>
       </c>
@@ -2141,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>79</v>
       </c>
@@ -2170,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>79</v>
       </c>
@@ -2199,7 +2191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -2228,7 +2220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>79</v>
       </c>
@@ -2257,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>79</v>
       </c>
@@ -2286,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>79</v>
       </c>
@@ -2315,7 +2307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>79</v>
       </c>
@@ -2344,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>79</v>
       </c>
@@ -2364,7 +2356,7 @@
         <v>4</v>
       </c>
       <c r="I32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J32" t="s">
         <v>0</v>
@@ -2373,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>79</v>
       </c>
@@ -2402,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>79</v>
       </c>
@@ -2422,7 +2414,7 @@
         <v>4</v>
       </c>
       <c r="I34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J34" t="s">
         <v>0</v>
@@ -2431,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -2451,7 +2443,7 @@
         <v>4</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J35" t="s">
         <v>0</v>
@@ -2460,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -2480,7 +2472,7 @@
         <v>4</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J36" t="s">
         <v>0</v>
@@ -2489,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>79</v>
       </c>
@@ -2518,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>79</v>
       </c>
@@ -2547,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>79</v>
       </c>
@@ -2576,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>79</v>
       </c>
@@ -2605,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>79</v>
       </c>
@@ -2625,7 +2617,7 @@
         <v>4</v>
       </c>
       <c r="I41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J41" t="s">
         <v>0</v>
@@ -2634,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -2654,7 +2646,7 @@
         <v>4</v>
       </c>
       <c r="I42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J42" t="s">
         <v>0</v>
@@ -2663,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>79</v>
       </c>
@@ -2683,7 +2675,7 @@
         <v>4</v>
       </c>
       <c r="I43">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J43" t="s">
         <v>0</v>
@@ -2692,7 +2684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>79</v>
       </c>
@@ -2712,7 +2704,7 @@
         <v>4</v>
       </c>
       <c r="I44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J44" t="s">
         <v>0</v>
@@ -2721,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>79</v>
       </c>
@@ -2741,7 +2733,7 @@
         <v>4</v>
       </c>
       <c r="I45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J45" t="s">
         <v>0</v>
@@ -2750,7 +2742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>79</v>
       </c>
@@ -2770,7 +2762,7 @@
         <v>4</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J46" t="s">
         <v>0</v>
@@ -2790,25 +2782,25 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B36" sqref="B7:B36"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -2843,7 +2835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -2876,7 +2868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -2905,12 +2897,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2945,7 +2937,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -2974,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -3003,7 +2995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>79</v>
       </c>
@@ -3032,7 +3024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -3061,7 +3053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -3090,7 +3082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -3119,7 +3111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -3148,7 +3140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -3177,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -3206,7 +3198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>79</v>
       </c>
@@ -3235,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>79</v>
       </c>
@@ -3264,7 +3256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>79</v>
       </c>
@@ -3293,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -3322,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>79</v>
       </c>
@@ -3351,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>79</v>
       </c>
@@ -3380,7 +3372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -3409,7 +3401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>79</v>
       </c>
@@ -3438,7 +3430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>79</v>
       </c>
@@ -3467,7 +3459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>79</v>
       </c>
@@ -3496,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>79</v>
       </c>
@@ -3525,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -3554,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>79</v>
       </c>
@@ -3583,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>79</v>
       </c>
@@ -3612,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>79</v>
       </c>
@@ -3641,7 +3633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>79</v>
       </c>
@@ -3670,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>79</v>
       </c>
@@ -3699,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>79</v>
       </c>
@@ -3728,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>79</v>
       </c>
@@ -3757,7 +3749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -3786,7 +3778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -3829,22 +3821,22 @@
       <selection activeCell="B7" sqref="B7:B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -3879,7 +3871,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -3912,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -3941,12 +3933,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -3981,7 +3973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -4004,7 +3996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -4027,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>79</v>
       </c>
@@ -4050,7 +4042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -4073,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -4096,7 +4088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -4119,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -4142,7 +4134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -4165,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -4188,7 +4180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>79</v>
       </c>
@@ -4211,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>79</v>
       </c>
@@ -4234,7 +4226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>79</v>
       </c>
@@ -4257,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -4280,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>79</v>
       </c>
@@ -4303,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>79</v>
       </c>
@@ -4326,7 +4318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>79</v>
       </c>
@@ -4349,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>79</v>
       </c>
@@ -4372,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>79</v>
       </c>
@@ -4395,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>79</v>
       </c>
@@ -4418,7 +4410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>79</v>
       </c>
@@ -4441,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>79</v>
       </c>
@@ -4464,7 +4456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>79</v>
       </c>
@@ -4487,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>79</v>
       </c>
@@ -4510,7 +4502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>79</v>
       </c>
@@ -4533,7 +4525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>79</v>
       </c>
@@ -4556,7 +4548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>79</v>
       </c>
@@ -4579,7 +4571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>79</v>
       </c>
@@ -4602,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>79</v>
       </c>
@@ -4625,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>79</v>
       </c>
@@ -4648,7 +4640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>79</v>
       </c>
@@ -4671,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>79</v>
       </c>
@@ -4694,7 +4686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>79</v>
       </c>
@@ -4717,7 +4709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>79</v>
       </c>
@@ -4740,7 +4732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>79</v>
       </c>
@@ -4763,7 +4755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>79</v>
       </c>
@@ -4786,7 +4778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>79</v>
       </c>
@@ -4809,7 +4801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>79</v>
       </c>
@@ -4832,7 +4824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>79</v>
       </c>
@@ -4855,7 +4847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>79</v>
       </c>
@@ -4878,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>79</v>
       </c>
@@ -4915,22 +4907,22 @@
       <selection activeCell="B21" sqref="B7:B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -4965,7 +4957,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -4998,7 +4990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -5027,12 +5019,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -5067,7 +5059,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -5084,7 +5076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -5101,7 +5093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>79</v>
       </c>
@@ -5118,7 +5110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -5135,7 +5127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>79</v>
       </c>
@@ -5152,7 +5144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>79</v>
       </c>
@@ -5169,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>79</v>
       </c>
@@ -5186,7 +5178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>79</v>
       </c>
@@ -5203,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>79</v>
       </c>
@@ -5220,7 +5212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>79</v>
       </c>
@@ -5237,7 +5229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>79</v>
       </c>
@@ -5254,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>79</v>
       </c>
@@ -5271,7 +5263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>79</v>
       </c>
@@ -5288,7 +5280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>79</v>
       </c>
@@ -5305,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>79</v>
       </c>
@@ -5336,22 +5328,22 @@
       <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -5386,7 +5378,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -5419,7 +5411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -5448,12 +5440,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -5488,7 +5480,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>79</v>
       </c>
@@ -5505,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>79</v>
       </c>
@@ -5522,7 +5514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>79</v>
       </c>
@@ -5539,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>79</v>
       </c>
@@ -5556,7 +5548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>79</v>
       </c>
@@ -5573,7 +5565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>79</v>
       </c>
@@ -5590,7 +5582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>79</v>
       </c>
@@ -5607,7 +5599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>79</v>
       </c>
@@ -5624,7 +5616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>79</v>
       </c>
@@ -5641,7 +5633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>79</v>
       </c>
@@ -5658,7 +5650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>79</v>
       </c>
@@ -5675,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>79</v>
       </c>
@@ -5692,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>79</v>
       </c>
@@ -5709,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>79</v>
       </c>
@@ -5726,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>79</v>
       </c>
@@ -5743,7 +5735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>79</v>
       </c>
@@ -5760,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>79</v>
       </c>
@@ -5777,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>79</v>
       </c>
@@ -5794,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
         <v>79</v>
       </c>
@@ -5811,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>79</v>
       </c>
@@ -5843,22 +5835,22 @@
       <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -5893,7 +5885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -5926,7 +5918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -5955,12 +5947,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -5995,7 +5987,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>83</v>
       </c>
@@ -6015,7 +6007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>83</v>
       </c>
@@ -6035,7 +6027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>83</v>
       </c>
@@ -6055,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>83</v>
       </c>
@@ -6075,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>83</v>
       </c>
@@ -6095,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>83</v>
       </c>
@@ -6115,7 +6107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>83</v>
       </c>
@@ -6135,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>83</v>
       </c>
@@ -6155,7 +6147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>83</v>
       </c>
@@ -6175,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>83</v>
       </c>
@@ -6195,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>83</v>
       </c>
@@ -6215,7 +6207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>83</v>
       </c>
@@ -6235,7 +6227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>83</v>
       </c>
@@ -6255,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>83</v>
       </c>
@@ -6275,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>83</v>
       </c>
@@ -6295,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>83</v>
       </c>
@@ -6315,7 +6307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>83</v>
       </c>
@@ -6335,7 +6327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>83</v>
       </c>
@@ -6355,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
         <v>83</v>
       </c>
@@ -6375,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>83</v>
       </c>
@@ -6395,7 +6387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
         <v>83</v>
       </c>
@@ -6415,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="11" t="s">
         <v>83</v>
       </c>
@@ -6435,7 +6427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
         <v>83</v>
       </c>
@@ -6455,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="11" t="s">
         <v>83</v>
       </c>
@@ -6475,7 +6467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="11" t="s">
         <v>83</v>
       </c>
@@ -6495,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
         <v>83</v>
       </c>
@@ -6515,7 +6507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="11" t="s">
         <v>83</v>
       </c>
@@ -6535,7 +6527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="11" t="s">
         <v>83</v>
       </c>
@@ -6555,7 +6547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="11" t="s">
         <v>83</v>
       </c>
@@ -6575,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
         <v>83</v>
       </c>
@@ -6595,25 +6587,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="11"/>
     </row>
-    <row r="38" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="11"/>
     </row>
-    <row r="39" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="11"/>
     </row>
-    <row r="40" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="11"/>
     </row>
-    <row r="41" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="11"/>
     </row>
-    <row r="42" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="11"/>
     </row>
-    <row r="43" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="11"/>
     </row>
   </sheetData>
@@ -6631,22 +6623,22 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -6681,7 +6673,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -6714,7 +6706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -6743,12 +6735,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -6783,7 +6775,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>85</v>
       </c>
@@ -6812,7 +6804,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>85</v>
       </c>
@@ -6841,7 +6833,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>85</v>
       </c>
@@ -6870,7 +6862,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>85</v>
       </c>
@@ -6899,7 +6891,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>85</v>
       </c>
@@ -6928,7 +6920,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>85</v>
       </c>
@@ -6957,7 +6949,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>85</v>
       </c>
@@ -6986,7 +6978,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>85</v>
       </c>
@@ -7015,7 +7007,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>85</v>
       </c>
@@ -7044,7 +7036,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>85</v>
       </c>
@@ -7073,7 +7065,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>85</v>
       </c>
@@ -7102,7 +7094,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>85</v>
       </c>
@@ -7131,7 +7123,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>85</v>
       </c>
@@ -7160,7 +7152,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>85</v>
       </c>
@@ -7189,7 +7181,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>85</v>
       </c>
@@ -7218,7 +7210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>85</v>
       </c>
@@ -7247,7 +7239,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>85</v>
       </c>
@@ -7276,7 +7268,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>85</v>
       </c>
@@ -7305,7 +7297,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
         <v>85</v>
       </c>
@@ -7334,7 +7326,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>85</v>
       </c>
@@ -7373,26 +7365,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23749389-52B3-407A-B3F2-AB9CC882FBFC}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D9" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="29.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -7427,7 +7419,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>69</v>
@@ -7460,7 +7452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>70</v>
@@ -7489,12 +7481,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -7529,7 +7521,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>86</v>
       </c>
@@ -7552,7 +7544,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>87</v>
       </c>
@@ -7575,7 +7567,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>86</v>
       </c>
@@ -7598,7 +7590,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>87</v>
       </c>
@@ -7621,7 +7613,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>86</v>
       </c>
@@ -7644,7 +7636,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>87</v>
       </c>
@@ -7667,7 +7659,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>86</v>
       </c>
@@ -7690,7 +7682,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="s">
         <v>87</v>
       </c>
@@ -7713,7 +7705,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="11" t="s">
         <v>86</v>
       </c>
@@ -7736,7 +7728,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="11" t="s">
         <v>87</v>
       </c>
@@ -7759,7 +7751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
         <v>86</v>
       </c>
@@ -7782,7 +7774,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>87</v>
       </c>
@@ -7805,7 +7797,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>86</v>
       </c>
@@ -7828,7 +7820,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>87</v>
       </c>
@@ -7851,7 +7843,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>86</v>
       </c>
@@ -7874,7 +7866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>87</v>
       </c>
@@ -7897,7 +7889,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>86</v>
       </c>
@@ -7920,7 +7912,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>87</v>
       </c>
@@ -7943,7 +7935,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
         <v>86</v>
       </c>
@@ -7966,7 +7958,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>87</v>
       </c>
@@ -7989,7 +7981,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
         <v>86</v>
       </c>
@@ -8012,7 +8004,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="11" t="s">
         <v>86</v>
       </c>
@@ -8035,7 +8027,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
         <v>87</v>
       </c>
@@ -8058,7 +8050,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="11" t="s">
         <v>86</v>
       </c>
@@ -8081,7 +8073,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="11" t="s">
         <v>87</v>
       </c>
@@ -8104,7 +8096,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
         <v>86</v>
       </c>
@@ -8127,7 +8119,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="11" t="s">
         <v>87</v>
       </c>
@@ -8150,7 +8142,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="11" t="s">
         <v>86</v>
       </c>
@@ -8173,7 +8165,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="11" t="s">
         <v>87</v>
       </c>
@@ -8196,7 +8188,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
         <v>86</v>
       </c>
@@ -8219,7 +8211,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>87</v>
       </c>
@@ -8242,7 +8234,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="11" t="s">
         <v>86</v>
       </c>
@@ -8265,7 +8257,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>87</v>
       </c>
@@ -8288,7 +8280,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
         <v>86</v>
       </c>
@@ -8311,7 +8303,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="11" t="s">
         <v>87</v>
       </c>
@@ -8334,7 +8326,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="11" t="s">
         <v>86</v>
       </c>
@@ -8357,7 +8349,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="11" t="s">
         <v>87</v>
       </c>
@@ -8380,7 +8372,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
         <v>86</v>
       </c>
@@ -8403,7 +8395,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="11" t="s">
         <v>87</v>
       </c>
@@ -8426,7 +8418,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="s">
         <v>86</v>
       </c>

</xml_diff>